<commit_message>
Update zu Gebäude und Wärmepumpe:
Gebäude:
WRG hinzugefügt
Wärmepumpe:
GUI-Update
Eingabe von variablen COP nun möglich
</commit_message>
<xml_diff>
--- a/EMS-Backend/data/building.xlsx
+++ b/EMS-Backend/data/building.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="9525" yWindow="2325" windowWidth="18810" windowHeight="9510" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="params" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="thermal_hull" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" calcMode="manual" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" calcMode="manual" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -421,10 +421,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -516,11 +516,26 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>€/m²BGF</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WRG</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>75</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>%</t>
         </is>
       </c>
     </row>
@@ -536,10 +551,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -579,58 +594,69 @@
         <v>1400</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>Boden</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>800</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.15</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>Dach</t>
         </is>
-      </c>
-      <c r="B4" t="n">
-        <v>800</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.4</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Fenster</t>
-        </is>
+      <c r="A5" t="n">
+        <v>800</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Fenster</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>